<commit_message>
Apex upload and table
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Seawater_chemistry/Seawater_samples.xlsx
+++ b/RAnalysis/Data/Seawater_chemistry/Seawater_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Pmagellanicus_omics\RAnalysis\Data\Seawater_chemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D139222D-964D-4E65-B5A6-0D23859D1913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D19B4B8-7017-41C6-87C8-E61C0F6AC226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{25AEC233-5A1B-46F0-BEA9-2D6D24EC308E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="104">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -733,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAD77E1-17A8-4A76-9D84-24AB1B149C99}">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -744,8 +744,8 @@
     <col min="3" max="3" width="5.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="95.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -767,10 +767,10 @@
         <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>26</v>
@@ -1144,10 +1144,10 @@
         <v>7</v>
       </c>
       <c r="F26" s="1">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G26" s="1">
         <v>7.63</v>
-      </c>
-      <c r="G26" s="1">
-        <v>8.6999999999999993</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>27</v>
@@ -1173,10 +1173,10 @@
         <v>10</v>
       </c>
       <c r="F27" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="G27" s="1">
         <v>7.45</v>
-      </c>
-      <c r="G27" s="1">
-        <v>12.7</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>27</v>
@@ -1202,10 +1202,10 @@
         <v>12</v>
       </c>
       <c r="F28" s="1">
+        <v>12.9</v>
+      </c>
+      <c r="G28" s="1">
         <v>7.58</v>
-      </c>
-      <c r="G28" s="1">
-        <v>12.9</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>27</v>
@@ -1231,10 +1231,10 @@
         <v>11</v>
       </c>
       <c r="F29" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G29" s="1">
         <v>7.59</v>
-      </c>
-      <c r="G29" s="1">
-        <v>8.8000000000000007</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>27</v>
@@ -1259,7 +1259,7 @@
       <c r="E30" s="1">
         <v>1</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>7.56</v>
       </c>
       <c r="I30" t="s">
@@ -1282,7 +1282,7 @@
       <c r="E31" s="1">
         <v>2</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>7.58</v>
       </c>
       <c r="I31" t="s">
@@ -1305,7 +1305,7 @@
       <c r="E32" s="1">
         <v>3</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>7.6</v>
       </c>
       <c r="I32" t="s">
@@ -1328,7 +1328,7 @@
       <c r="E33" s="1">
         <v>4</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>7.54</v>
       </c>
       <c r="I33" t="s">
@@ -1351,7 +1351,7 @@
       <c r="E34" s="1">
         <v>5</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>7.52</v>
       </c>
       <c r="I34" t="s">
@@ -1374,7 +1374,7 @@
       <c r="E35" s="1">
         <v>6</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>7.58</v>
       </c>
       <c r="I35" t="s">
@@ -1397,7 +1397,7 @@
       <c r="E36" s="1">
         <v>7</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>7.54</v>
       </c>
       <c r="I36" t="s">
@@ -1420,7 +1420,7 @@
       <c r="E37" s="1">
         <v>8</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>7.59</v>
       </c>
       <c r="I37" t="s">
@@ -1443,7 +1443,7 @@
       <c r="E38" s="1">
         <v>9</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>7.72</v>
       </c>
       <c r="I38" t="s">
@@ -1466,7 +1466,7 @@
       <c r="E39" s="1">
         <v>10</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>7.71</v>
       </c>
       <c r="I39" t="s">
@@ -1489,7 +1489,7 @@
       <c r="E40" s="1">
         <v>11</v>
       </c>
-      <c r="F40" s="1">
+      <c r="G40" s="1">
         <v>7.58</v>
       </c>
       <c r="I40" t="s">
@@ -1512,7 +1512,7 @@
       <c r="E41" s="1">
         <v>12</v>
       </c>
-      <c r="F41" s="1">
+      <c r="G41" s="1">
         <v>7.58</v>
       </c>
       <c r="I41" t="s">
@@ -1535,7 +1535,7 @@
       <c r="E42" s="1">
         <v>13</v>
       </c>
-      <c r="F42" s="1">
+      <c r="G42" s="1">
         <v>7.57</v>
       </c>
       <c r="I42" t="s">
@@ -1558,7 +1558,7 @@
       <c r="E43" s="1">
         <v>14</v>
       </c>
-      <c r="F43" s="1">
+      <c r="G43" s="1">
         <v>7.58</v>
       </c>
       <c r="I43" t="s">
@@ -1581,7 +1581,7 @@
       <c r="E44" s="1">
         <v>15</v>
       </c>
-      <c r="F44" s="1">
+      <c r="G44" s="1">
         <v>7.7</v>
       </c>
       <c r="I44" t="s">
@@ -1625,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="F46" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="G46" s="1">
         <v>7.6</v>
-      </c>
-      <c r="G46" s="1">
-        <v>10.7</v>
       </c>
       <c r="I46" t="s">
         <v>35</v>
@@ -1651,10 +1651,10 @@
         <v>5</v>
       </c>
       <c r="F47" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="G47" s="1">
         <v>7.61</v>
-      </c>
-      <c r="G47" s="1">
-        <v>14.6</v>
       </c>
       <c r="I47" t="s">
         <v>35</v>
@@ -1677,10 +1677,10 @@
         <v>9</v>
       </c>
       <c r="F48" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="G48" s="1">
         <v>7.85</v>
-      </c>
-      <c r="G48" s="1">
-        <v>14.6</v>
       </c>
       <c r="I48" t="s">
         <v>36</v>
@@ -1703,10 +1703,10 @@
         <v>13</v>
       </c>
       <c r="F49" s="1">
+        <v>14.4</v>
+      </c>
+      <c r="G49" s="1">
         <v>7.64</v>
-      </c>
-      <c r="G49" s="1">
-        <v>14.4</v>
       </c>
       <c r="I49" t="s">
         <v>36</v>
@@ -1716,153 +1716,489 @@
       <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="B50" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D50" s="1">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>9.6</v>
+      </c>
+      <c r="G50">
+        <v>7.52</v>
+      </c>
+      <c r="I50" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="B51" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D51" s="1">
+        <v>10</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>14.7</v>
+      </c>
+      <c r="G51">
+        <v>7.52</v>
+      </c>
+      <c r="I51" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="B52" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D52" s="1">
+        <v>10</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3</v>
+      </c>
+      <c r="F52">
+        <v>14.8</v>
+      </c>
+      <c r="G52">
+        <v>7.69</v>
+      </c>
+      <c r="I52" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="B53" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D53" s="1">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4</v>
+      </c>
+      <c r="F53">
+        <v>9.5</v>
+      </c>
+      <c r="G53">
+        <v>7.68</v>
+      </c>
+      <c r="I53" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="B54" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D54" s="1">
+        <v>10</v>
+      </c>
+      <c r="E54" s="1">
+        <v>5</v>
+      </c>
+      <c r="F54">
+        <v>14.8</v>
+      </c>
+      <c r="G54">
+        <v>7.55</v>
+      </c>
+      <c r="I54" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="B55" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D55" s="1">
+        <v>10</v>
+      </c>
+      <c r="E55" s="1">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>9.4</v>
+      </c>
+      <c r="G55">
+        <v>7.74</v>
+      </c>
+      <c r="I55" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="B56" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D56" s="1">
+        <v>10</v>
+      </c>
+      <c r="E56" s="1">
+        <v>7</v>
+      </c>
+      <c r="F56">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="G56">
+        <v>7.51</v>
+      </c>
+      <c r="I56" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="B57" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D57" s="1">
+        <v>10</v>
+      </c>
+      <c r="E57" s="1">
+        <v>8</v>
+      </c>
+      <c r="F57">
+        <v>14.6</v>
+      </c>
+      <c r="G57">
+        <v>7.67</v>
+      </c>
+      <c r="I57" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="B58" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D58" s="1">
+        <v>10</v>
+      </c>
+      <c r="E58" s="1">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>14.6</v>
+      </c>
+      <c r="G58">
+        <v>7.7</v>
+      </c>
+      <c r="I58" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>82</v>
       </c>
+      <c r="B59" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D59" s="1">
+        <v>10</v>
+      </c>
+      <c r="E59" s="1">
+        <v>10</v>
+      </c>
+      <c r="F59">
+        <v>14.6</v>
+      </c>
+      <c r="G59">
+        <v>7.67</v>
+      </c>
+      <c r="I59" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="B60" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D60" s="1">
+        <v>10</v>
+      </c>
+      <c r="E60" s="1">
+        <v>11</v>
+      </c>
+      <c r="F60">
+        <v>9.1</v>
+      </c>
+      <c r="G60">
+        <v>7.66</v>
+      </c>
+      <c r="I60" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>84</v>
       </c>
+      <c r="B61" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D61" s="1">
+        <v>10</v>
+      </c>
+      <c r="E61" s="1">
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <v>14.8</v>
+      </c>
+      <c r="G61">
+        <v>7.58</v>
+      </c>
+      <c r="I61" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>85</v>
       </c>
+      <c r="B62" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D62" s="1">
+        <v>10</v>
+      </c>
+      <c r="E62" s="1">
+        <v>13</v>
+      </c>
+      <c r="F62">
+        <v>14.5</v>
+      </c>
+      <c r="G62">
+        <v>7.56</v>
+      </c>
+      <c r="I62" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="B63" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D63" s="1">
+        <v>10</v>
+      </c>
+      <c r="E63" s="1">
+        <v>14</v>
+      </c>
+      <c r="F63">
+        <v>8.9</v>
+      </c>
+      <c r="G63">
+        <v>7.54</v>
+      </c>
+      <c r="I63" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B64" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D64" s="1">
+        <v>10</v>
+      </c>
+      <c r="E64" s="1">
+        <v>15</v>
+      </c>
+      <c r="F64">
+        <v>8.9</v>
+      </c>
+      <c r="G64">
+        <v>7.66</v>
+      </c>
+      <c r="I64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B65" s="1">
+        <v>20250622</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D65" s="1">
+        <v>10</v>
+      </c>
+      <c r="E65" s="1">
+        <v>16</v>
+      </c>
+      <c r="F65">
+        <v>8.9</v>
+      </c>
+      <c r="G65">
+        <v>7.51</v>
+      </c>
+      <c r="I65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
updated data and sw chem script
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Seawater_chemistry/Seawater_samples.xlsx
+++ b/RAnalysis/Data/Seawater_chemistry/Seawater_samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Pmagellanicus_omics\RAnalysis\Data\Seawater_chemistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D0DFC-2A24-48AE-85D0-734A20009E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C26A2-D38A-49E9-ADFB-2EA8D3589925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{25AEC233-5A1B-46F0-BEA9-2D6D24EC308E}"/>
+    <workbookView xWindow="-14235" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{25AEC233-5A1B-46F0-BEA9-2D6D24EC308E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAAD77E1-17A8-4A76-9D84-24AB1B149C99}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,6 +859,7 @@
       <c r="F4" s="3">
         <v>31.45</v>
       </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="2" t="s">
         <v>23</v>
       </c>
@@ -882,6 +883,7 @@
       <c r="F5" s="3">
         <v>31.45</v>
       </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="2" t="s">
         <v>23</v>
       </c>
@@ -2678,6 +2680,12 @@
       <c r="F66" s="1">
         <v>31.56</v>
       </c>
+      <c r="G66">
+        <v>15</v>
+      </c>
+      <c r="H66">
+        <v>7.86</v>
+      </c>
       <c r="I66" s="2" t="s">
         <v>23</v>
       </c>
@@ -2701,6 +2709,12 @@
       <c r="F67" s="1">
         <v>31.56</v>
       </c>
+      <c r="G67">
+        <v>15.2</v>
+      </c>
+      <c r="H67">
+        <v>7.6</v>
+      </c>
       <c r="I67" s="2" t="s">
         <v>23</v>
       </c>
@@ -2724,6 +2738,12 @@
       <c r="F68" s="1">
         <v>31.56</v>
       </c>
+      <c r="G68">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H68">
+        <v>7.78</v>
+      </c>
       <c r="I68" s="2" t="s">
         <v>23</v>
       </c>
@@ -2747,6 +2767,12 @@
       <c r="F69" s="1">
         <v>31.56</v>
       </c>
+      <c r="G69">
+        <v>8.9</v>
+      </c>
+      <c r="H69">
+        <v>7.65</v>
+      </c>
       <c r="I69" s="2" t="s">
         <v>23</v>
       </c>
@@ -2770,6 +2796,12 @@
       <c r="F70" s="2">
         <v>31.63</v>
       </c>
+      <c r="G70">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H70">
+        <v>7.55</v>
+      </c>
       <c r="I70" s="2" t="s">
         <v>23</v>
       </c>
@@ -2796,6 +2828,12 @@
       <c r="F71" s="2">
         <v>31.63</v>
       </c>
+      <c r="G71">
+        <v>15.1</v>
+      </c>
+      <c r="H71">
+        <v>7.59</v>
+      </c>
       <c r="I71" s="2" t="s">
         <v>23</v>
       </c>
@@ -2822,6 +2860,12 @@
       <c r="F72" s="2">
         <v>31.63</v>
       </c>
+      <c r="G72">
+        <v>15.2</v>
+      </c>
+      <c r="H72">
+        <v>7.74</v>
+      </c>
       <c r="I72" s="2" t="s">
         <v>23</v>
       </c>
@@ -2848,6 +2892,12 @@
       <c r="F73" s="2">
         <v>31.63</v>
       </c>
+      <c r="G73">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H73">
+        <v>7.65</v>
+      </c>
       <c r="I73" s="2" t="s">
         <v>23</v>
       </c>
@@ -2874,6 +2924,12 @@
       <c r="F74" s="2">
         <v>31.63</v>
       </c>
+      <c r="G74">
+        <v>15.1</v>
+      </c>
+      <c r="H74">
+        <v>7.58</v>
+      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
@@ -2894,6 +2950,12 @@
       <c r="F75" s="2">
         <v>31.63</v>
       </c>
+      <c r="G75">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H75">
+        <v>7.69</v>
+      </c>
       <c r="J75" s="2" t="s">
         <v>86</v>
       </c>
@@ -2917,6 +2979,12 @@
       <c r="F76" s="2">
         <v>31.63</v>
       </c>
+      <c r="G76">
+        <v>9.1</v>
+      </c>
+      <c r="H76">
+        <v>7.61</v>
+      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
@@ -2937,6 +3005,12 @@
       <c r="F77" s="2">
         <v>31.63</v>
       </c>
+      <c r="G77">
+        <v>15</v>
+      </c>
+      <c r="H77">
+        <v>7.77</v>
+      </c>
       <c r="J77" s="2" t="s">
         <v>86</v>
       </c>
@@ -2960,6 +3034,12 @@
       <c r="F78" s="2">
         <v>31.63</v>
       </c>
+      <c r="G78">
+        <v>15.1</v>
+      </c>
+      <c r="H78">
+        <v>7.75</v>
+      </c>
       <c r="J78" s="2" t="s">
         <v>86</v>
       </c>
@@ -2983,6 +3063,12 @@
       <c r="F79" s="2">
         <v>31.63</v>
       </c>
+      <c r="G79">
+        <v>15</v>
+      </c>
+      <c r="H79">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
@@ -3003,6 +3089,12 @@
       <c r="F80" s="2">
         <v>31.63</v>
       </c>
+      <c r="G80">
+        <v>9.4</v>
+      </c>
+      <c r="H80">
+        <v>7.71</v>
+      </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
@@ -3023,6 +3115,12 @@
       <c r="F81" s="2">
         <v>31.63</v>
       </c>
+      <c r="G81">
+        <v>15.3</v>
+      </c>
+      <c r="H81">
+        <v>7.62</v>
+      </c>
       <c r="J81" s="2" t="s">
         <v>86</v>
       </c>
@@ -3046,6 +3144,12 @@
       <c r="F82" s="2">
         <v>31.63</v>
       </c>
+      <c r="G82">
+        <v>14.9</v>
+      </c>
+      <c r="H82">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
@@ -3066,6 +3170,12 @@
       <c r="F83" s="2">
         <v>31.63</v>
       </c>
+      <c r="G83">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H83">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
@@ -3086,6 +3196,12 @@
       <c r="F84" s="2">
         <v>31.63</v>
       </c>
+      <c r="G84">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="H84">
+        <v>7.68</v>
+      </c>
       <c r="J84" s="2" t="s">
         <v>86</v>
       </c>
@@ -3108,6 +3224,12 @@
       </c>
       <c r="F85" s="2">
         <v>31.63</v>
+      </c>
+      <c r="G85">
+        <v>9.4</v>
+      </c>
+      <c r="H85">
+        <v>7.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>